<commit_message>
UI-820: Updated skeleton Test Plan
</commit_message>
<xml_diff>
--- a/apps/skeleton/design/Test Plan/TestPlan.xlsx
+++ b/apps/skeleton/design/Test Plan/TestPlan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>Application Name</t>
   </si>
@@ -100,9 +100,6 @@
     <t>This app was created to allow Monster-UI Users to …</t>
   </si>
   <si>
-    <t>% Link to a document, explaining the requirements to test this application, if it needs some %</t>
-  </si>
-  <si>
     <t>If your app has some weird behavior, try to explain it here, otherwise leave it blank</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
   </si>
   <si>
     <t>….</t>
+  </si>
+  <si>
+    <t>List the roles here. We only have 3 roles In Monster-UI : Standard Account, Reseller and Superduper. Please specify Reseller/Superduper only if your app has some special edge cases involving a Reseller/Superduper account</t>
   </si>
 </sst>
 </file>
@@ -155,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,27 +185,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -225,8 +211,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -369,17 +367,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -395,11 +382,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -410,223 +396,206 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -937,7 +906,7 @@
   <dimension ref="B2:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -958,102 +927,102 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="35"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="46"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="51"/>
+      <c r="D3" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="13">
+      <c r="C4" s="53"/>
+      <c r="D4" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="14" t="s">
+      <c r="C5" s="55"/>
+      <c r="D5" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="22" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="48"/>
+      <c r="D8" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="2:10" s="3" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="26" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C10" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="68">
+        <v>1</v>
+      </c>
+      <c r="D11" s="69" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C10" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="27">
-        <v>1</v>
-      </c>
-      <c r="D11" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="7"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
+      <c r="I11" s="70"/>
+      <c r="J11" s="71"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="E12" s="38" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="40" t="s">
@@ -1061,135 +1030,145 @@
       </c>
       <c r="G12" s="41"/>
       <c r="H12" s="41"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="36" t="s">
+      <c r="I12" s="38"/>
+      <c r="J12" s="42" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="54"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="15" t="s">
+      <c r="C13" s="49"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="G13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J13" s="37"/>
+      <c r="J13" s="43"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="72" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="56"/>
-      <c r="H14" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="11"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="9"/>
     </row>
     <row r="15" spans="2:10" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="65" t="s">
+      <c r="D15" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="73" t="s">
+      <c r="E15" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="67"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="69" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="70"/>
-      <c r="J15" s="71"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="62"/>
     </row>
     <row r="16" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C16" s="55" t="s">
+      <c r="C16" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="64" t="s">
+      <c r="D16" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="74" t="s">
+      <c r="E16" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="25"/>
-      <c r="J16" s="9"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="58" t="s">
+      <c r="E17" s="58" t="s">
         <v>36</v>
-      </c>
-      <c r="E17" s="75" t="s">
-        <v>37</v>
       </c>
       <c r="F17" s="59"/>
       <c r="G17" s="60"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="61"/>
+      <c r="H17" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="61" t="s">
+        <v>22</v>
+      </c>
       <c r="J17" s="62"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C20" s="27">
+      <c r="C20" s="68">
         <v>1</v>
       </c>
-      <c r="D20" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="7"/>
+      <c r="D20" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="70"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="70"/>
+      <c r="H20" s="70"/>
+      <c r="I20" s="70"/>
+      <c r="J20" s="71"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C21" s="43" t="s">
+      <c r="C21" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="38" t="s">
         <v>7</v>
       </c>
       <c r="F21" s="40" t="s">
@@ -1197,102 +1176,91 @@
       </c>
       <c r="G21" s="41"/>
       <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="36" t="s">
+      <c r="I21" s="38"/>
+      <c r="J21" s="42" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C22" s="44"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="15" t="s">
+      <c r="C22" s="35"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="H22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J22" s="37"/>
+      <c r="J22" s="43"/>
     </row>
     <row r="23" spans="3:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="72" t="s">
+      <c r="D23" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="9"/>
+    </row>
+    <row r="24" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C24" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E24" s="66" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="59"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="61" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="62"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C25" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="J23" s="11"/>
-    </row>
-    <row r="24" spans="3:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="C24" s="76" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="73" t="s">
-        <v>39</v>
-      </c>
-      <c r="E24" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="67"/>
-      <c r="G24" s="77" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="69" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="71"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
-      <c r="C25" s="32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="74" t="s">
+      <c r="E25" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="J25" s="9"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="J21:J22"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="B6:C6"/>
@@ -1305,11 +1273,13 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="J21:J22"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" display="https://github.com/2600hz/monster-ui/blob/master/docs/testRequirements.md"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated skeleton's TestPlan to auto-increment the tests ID
</commit_message>
<xml_diff>
--- a/apps/skeleton/design/Test Plan/TestPlan.xlsx
+++ b/apps/skeleton/design/Test Plan/TestPlan.xlsx
@@ -425,109 +425,53 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -889,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,62 +855,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="26.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="37"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="37"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="35"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="16" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:10" s="3" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="35"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="17" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="35"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
@@ -987,6 +931,7 @@
     </row>
     <row r="11" spans="2:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="10">
+        <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
         <v>1</v>
       </c>
       <c r="D11" s="11" t="s">
@@ -1000,29 +945,29 @@
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="E12" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="32" t="s">
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="36"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="29"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="35"/>
       <c r="F13" s="7" t="s">
         <v>19</v>
       </c>
@@ -1035,7 +980,7 @@
       <c r="I13" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J13" s="33"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C14" s="18" t="str">
@@ -1137,7 +1082,8 @@
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C20" s="10">
-        <v>1</v>
+        <f ca="1">MAX(INDIRECT("C1:C"&amp;ROW()-1))+1</f>
+        <v>2</v>
       </c>
       <c r="D20" s="11" t="s">
         <v>32</v>
@@ -1150,29 +1096,29 @@
       <c r="J20" s="13"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="32" t="s">
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="25" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" spans="3:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="C22" s="25"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="29"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="35"/>
       <c r="F22" s="7" t="s">
         <v>19</v>
       </c>
@@ -1185,7 +1131,7 @@
       <c r="I22" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J22" s="33"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" spans="3:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C23" s="18" t="str">
@@ -1252,6 +1198,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="J21:J22"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="B6:C6"/>
@@ -1264,25 +1215,20 @@
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="J21:J22"/>
   </mergeCells>
   <conditionalFormatting sqref="F14:I17">
-    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",F14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",F14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23:I25">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",F23)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="F">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH("F",F23)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>